<commit_message>
Added Sample Test Case for Layer 4 5 6
</commit_message>
<xml_diff>
--- a/Symmetric_LSH/E2LSH-0.1/NBA_Sample_Test_Season_2017_2018/Sample_Result_Aggregation.xlsx
+++ b/Symmetric_LSH/E2LSH-0.1/NBA_Sample_Test_Season_2017_2018/Sample_Result_Aggregation.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sliu104/Desktop/StreamingTopK/Symmetric_LSH/E2LSH-0.1/NBA_Sample_Test_Season_2017_2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sicongliu/Desktop/StreamingTopK/Symmetric_LSH/E2LSH-0.1/NBA_Sample_Test_Season_2017_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1940" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2120" yWindow="900" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NBA_Data" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
   <si>
     <t>Layer_1</t>
   </si>
@@ -74,6 +74,18 @@
   <si>
     <t>Layer_Data_Index</t>
   </si>
+  <si>
+    <t>Layer_4</t>
+  </si>
+  <si>
+    <t>Layer_5</t>
+  </si>
+  <si>
+    <t>Layer_6</t>
+  </si>
+  <si>
+    <t>Top_50</t>
+  </si>
 </sst>
 </file>
 
@@ -111,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +133,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,7 +152,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -198,16 +216,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -239,6 +267,10 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -270,6 +302,10 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -548,7 +584,7 @@
   <dimension ref="A1:G530"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6402,15 +6438,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M275"/>
+  <dimension ref="A1:AB275"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView showRuler="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6438,8 +6474,35 @@
       <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6467,8 +6530,35 @@
       <c r="M2">
         <v>0.63609000000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0.75131700000000001</v>
+      </c>
+      <c r="R2">
+        <v>0.659941</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0.70710700000000004</v>
+      </c>
+      <c r="W2">
+        <v>0.70710700000000004</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0.70710700000000004</v>
+      </c>
+      <c r="AB2">
+        <v>0.70710700000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6496,8 +6586,35 @@
       <c r="M3">
         <v>0.63872200000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>0.77433700000000005</v>
+      </c>
+      <c r="R3">
+        <v>0.63277300000000003</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>0.76910800000000001</v>
+      </c>
+      <c r="W3">
+        <v>0.63911799999999996</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>0.76822100000000004</v>
+      </c>
+      <c r="AB3">
+        <v>0.64018399999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6525,8 +6642,35 @@
       <c r="M4">
         <v>0.63722800000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>0.77917999999999998</v>
+      </c>
+      <c r="R4">
+        <v>0.62680000000000002</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>0.76822100000000004</v>
+      </c>
+      <c r="W4">
+        <v>0.64018399999999998</v>
+      </c>
+      <c r="Z4">
+        <v>3</v>
+      </c>
+      <c r="AA4">
+        <v>0.83204999999999996</v>
+      </c>
+      <c r="AB4">
+        <v>0.55469999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6554,8 +6698,26 @@
       <c r="M5">
         <v>0.61785699999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>0.70710700000000004</v>
+      </c>
+      <c r="R5">
+        <v>0.70710700000000004</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>0.75230900000000001</v>
+      </c>
+      <c r="W5">
+        <v>0.65881000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6583,8 +6745,26 @@
       <c r="M6">
         <v>0.57680600000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>0.78057299999999996</v>
+      </c>
+      <c r="R6">
+        <v>0.62506399999999995</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="V6">
+        <v>0.83204999999999996</v>
+      </c>
+      <c r="W6">
+        <v>0.55469999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6612,8 +6792,26 @@
       <c r="M7">
         <v>0.66401699999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>0.76910800000000001</v>
+      </c>
+      <c r="R7">
+        <v>0.63911799999999996</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <v>0.75247799999999998</v>
+      </c>
+      <c r="W7">
+        <v>0.65861700000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6641,8 +6839,17 @@
       <c r="M8">
         <v>0.63938799999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8">
+        <v>0.83204999999999996</v>
+      </c>
+      <c r="R8">
+        <v>0.55469999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6670,8 +6877,17 @@
       <c r="M9">
         <v>0.62401600000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <v>8</v>
+      </c>
+      <c r="Q9">
+        <v>0.78014600000000001</v>
+      </c>
+      <c r="R9">
+        <v>0.62559699999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6699,8 +6915,17 @@
       <c r="M10">
         <v>0.67066499999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P10">
+        <v>9</v>
+      </c>
+      <c r="Q10">
+        <v>0.75087199999999998</v>
+      </c>
+      <c r="R10">
+        <v>0.66044700000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6728,8 +6953,17 @@
       <c r="M11">
         <v>0.64341199999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>0.76822100000000004</v>
+      </c>
+      <c r="R11">
+        <v>0.64018399999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6757,8 +6991,17 @@
       <c r="M12">
         <v>0.65552500000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P12">
+        <v>11</v>
+      </c>
+      <c r="Q12">
+        <v>0.76700500000000005</v>
+      </c>
+      <c r="R12">
+        <v>0.64164100000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6786,8 +7029,17 @@
       <c r="M13">
         <v>0.63311799999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P13">
+        <v>12</v>
+      </c>
+      <c r="Q13">
+        <v>0.76856400000000002</v>
+      </c>
+      <c r="R13">
+        <v>0.63977200000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6815,8 +7067,17 @@
       <c r="M14">
         <v>0.70710700000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P14">
+        <v>13</v>
+      </c>
+      <c r="Q14">
+        <v>0.78028699999999995</v>
+      </c>
+      <c r="R14">
+        <v>0.625421</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6844,8 +7105,17 @@
       <c r="M15">
         <v>0.68981000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P15">
+        <v>14</v>
+      </c>
+      <c r="Q15">
+        <v>0.77414300000000003</v>
+      </c>
+      <c r="R15">
+        <v>0.63300999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6873,8 +7143,17 @@
       <c r="M16">
         <v>0.60667300000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P16">
+        <v>15</v>
+      </c>
+      <c r="Q16">
+        <v>0.73848499999999895</v>
+      </c>
+      <c r="R16">
+        <v>0.67426900000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6902,8 +7181,17 @@
       <c r="M17">
         <v>0.66710899999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P17">
+        <v>16</v>
+      </c>
+      <c r="Q17">
+        <v>0.770903</v>
+      </c>
+      <c r="R17">
+        <v>0.63695199999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6931,8 +7219,17 @@
       <c r="M18">
         <v>0.56030899999999895</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P18">
+        <v>17</v>
+      </c>
+      <c r="Q18">
+        <v>0.75257700000000005</v>
+      </c>
+      <c r="R18">
+        <v>0.65850500000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6960,8 +7257,17 @@
       <c r="M19">
         <v>0.59173500000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P19">
+        <v>18</v>
+      </c>
+      <c r="Q19">
+        <v>0.758185</v>
+      </c>
+      <c r="R19">
+        <v>0.65203900000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6989,8 +7295,17 @@
       <c r="M20">
         <v>0.62700900000000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P20">
+        <v>19</v>
+      </c>
+      <c r="Q20">
+        <v>0.74329400000000001</v>
+      </c>
+      <c r="R20">
+        <v>0.66896500000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -7018,8 +7333,17 @@
       <c r="M21">
         <v>0.55469999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P21">
+        <v>20</v>
+      </c>
+      <c r="Q21">
+        <v>0.79178199999999999</v>
+      </c>
+      <c r="R21">
+        <v>0.61080299999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -7048,7 +7372,7 @@
         <v>0.64966299999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -7077,7 +7401,7 @@
         <v>0.609653</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -7106,7 +7430,7 @@
         <v>0.64706600000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -7135,7 +7459,7 @@
         <v>0.64018399999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -7164,7 +7488,7 @@
         <v>0.63284399999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -7193,7 +7517,7 @@
         <v>0.67743399999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -7222,7 +7546,7 @@
         <v>0.69078300000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -7251,7 +7575,7 @@
         <v>0.63656500000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -7280,7 +7604,7 @@
         <v>0.66896500000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -7309,7 +7633,7 @@
         <v>0.60520099999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -11413,10 +11737,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView showRuler="0" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12702,6 +13026,18 @@
         <v>0.43657699999999999</v>
       </c>
     </row>
+    <row r="38" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -12712,8 +13048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12748,6 +13084,9 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -12762,7 +13101,9 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
@@ -12777,7 +13118,9 @@
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
       <c r="P2" s="3" t="s">
         <v>4</v>
       </c>
@@ -13260,16 +13603,16 @@
       <c r="E15">
         <v>0.34821000000000002</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="5">
         <v>412</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="5">
         <v>0.56818999999999997</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="5">
         <v>0.82289999999999996</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="5">
         <v>0.22203000000000001</v>
       </c>
       <c r="P15">
@@ -13324,54 +13667,54 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17">
+      <c r="B17" s="4">
         <v>137</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>0.57801999999999998</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>0.81601999999999997</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>0.36001</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="5">
         <v>137</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="5">
         <v>0.57801999999999998</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="5">
         <v>0.81601999999999997</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="5">
         <v>0.23396</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="4">
         <v>137</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="4">
         <v>0.57801999999999998</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="4">
         <v>0.81601999999999997</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="4">
         <v>0.2228</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18">
+      <c r="B18" s="4">
         <v>71</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>0.58123999999999998</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>0.81372999999999995</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>0.3639</v>
       </c>
       <c r="I18" s="1">
@@ -13438,16 +13781,16 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20">
+      <c r="B20" s="4">
         <v>283</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>0.58611999999999997</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>0.81022000000000005</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>0.36981000000000003</v>
       </c>
       <c r="I20" s="1">

</xml_diff>